<commit_message>
add TA session 7
</commit_message>
<xml_diff>
--- a/slide_data_code_correspondence.xlsx
+++ b/slide_data_code_correspondence.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="158">
   <si>
     <t>auto</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -384,6 +384,306 @@
   </si>
   <si>
     <t>cases（follow the order it appears in slide）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree(Decision tree)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regression tree(eg.Baseball Salary)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean in the region as prediction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classification tree(eg.transport)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>most common case as predicion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>criteria in growing a tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>according to the class of y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y is contineous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y is discrete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[min RSS in training data]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[min E/ Gini index/ Cross Entropy in training data]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>both use a recursive binary splitting method in growing a tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic concepts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>advantage and disadvantge of tree method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>advantage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>②easy to handle qualitative explanatory variables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①low predictive accuracy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>②high variance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">disadvantge </t>
+  </si>
+  <si>
+    <t>single tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prune a tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build a tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>① easy to interprete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bootstrap+averaging+all X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random forest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bootstrap+averaging+subset of X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①tree (tree, cv.tree)
+②rpart(rpart,prune)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+①randomForest(randomForest)
+②ranger
+③caret(train)
+④h2o
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boosting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no bootstrap+sequentially learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①gbm (gbm)
+②caret(train)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example Demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logistic model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ——classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test error rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method to improve the performance of single tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pruned tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>randomforest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boosting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boosting is the best model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ——regression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linear model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging is the best model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>two Simulates in slides</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simulate 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not control the terminal node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>control the terminal node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> ——classification(true boundary is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> linear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logistic model_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> ——classification(true boundary is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>non-linear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linear boundry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>non-linear boundry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simulate 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tree-based model gives better model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polish bankruptcy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boston House Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R package(main functions)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no method can beat the logistica model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -391,7 +691,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +716,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +760,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -516,11 +855,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,6 +1017,82 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -894,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1421,14 +1927,566 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="41.21875" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="44"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="44"/>
+      <c r="C5" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="44"/>
+      <c r="C6" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="45"/>
+      <c r="C11" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="42"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+    </row>
+    <row r="20" spans="2:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
+      <c r="C20" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+    </row>
+    <row r="21" spans="2:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="2:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="31"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="32"/>
+      <c r="C28" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="41"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="53">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="53">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="D30" s="54"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="53">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="D31" s="54"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="55">
+        <v>5.21E-2</v>
+      </c>
+      <c r="D32" s="54"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="36"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="42"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="32"/>
+      <c r="C35" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="41"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="57">
+        <v>21.89855</v>
+      </c>
+      <c r="D36" s="54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="57">
+        <v>17.341989999999999</v>
+      </c>
+      <c r="D37" s="54"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="57">
+        <v>10.993679999999999</v>
+      </c>
+      <c r="D38" s="54"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="58">
+        <v>8.7883069999999996</v>
+      </c>
+      <c r="D39" s="54"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="57">
+        <v>9.0699480000000001</v>
+      </c>
+      <c r="D40" s="54"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="36"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="42"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="31"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="32"/>
+      <c r="C45" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="41"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="58">
+        <v>0.17330000000000001</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="57">
+        <v>0.22</v>
+      </c>
+      <c r="D47" s="54"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="57">
+        <v>0.2175</v>
+      </c>
+      <c r="D48" s="54"/>
+      <c r="E48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="57">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="D49" s="54"/>
+      <c r="E49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="57">
+        <v>0.1933</v>
+      </c>
+      <c r="D50" s="54"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="36"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="42"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="31"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="32"/>
+      <c r="C53" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="41"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="57">
+        <v>0.26666669999999998</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="57">
+        <v>0.12666669999999999</v>
+      </c>
+      <c r="D55" s="54"/>
+      <c r="E55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="57">
+        <v>0.14166670000000001</v>
+      </c>
+      <c r="D56" s="54"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="57">
+        <v>0.12333330000000001</v>
+      </c>
+      <c r="D57" s="54"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="58">
+        <v>0.105</v>
+      </c>
+      <c r="D58" s="54"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="60">
+        <v>0.1216667</v>
+      </c>
+      <c r="D59" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="E4:H11"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>